<commit_message>
initial azimuth calculation working
</commit_message>
<xml_diff>
--- a/CCP Trade Tree Analysis.xlsx
+++ b/CCP Trade Tree Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuitenbr/Desktop/lunarspark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E2C056-C6AC-C845-ADA6-B5217271B29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDD825F-851E-1E44-812E-300AF784F883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41960" yWindow="500" windowWidth="32220" windowHeight="21100" activeTab="2" xr2:uid="{0D0644B8-F9A6-4A61-A91E-2BD3522A7E9F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="4" xr2:uid="{0D0644B8-F9A6-4A61-A91E-2BD3522A7E9F}"/>
   </bookViews>
   <sheets>
     <sheet name="SE analysis" sheetId="1" r:id="rId1"/>
@@ -7986,7 +7986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB1BC88-0916-3A47-BF9E-DDA64C4AACEA}">
   <dimension ref="B3:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
@@ -10649,8 +10649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E790B1-52D8-A842-8268-804FFB128667}">
   <dimension ref="A2:Q56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12005,12 +12005,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56d601e6-bef3-45c8-b6dc-25c3b07e1d58">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12200,19 +12201,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56d601e6-bef3-45c8-b6dc-25c3b07e1d58">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5C6F309-A1A2-46F0-A57B-68684D972651}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7469B838-CC0E-428C-B339-A9883501F19C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="56d601e6-bef3-45c8-b6dc-25c3b07e1d58"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12236,11 +12238,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7469B838-CC0E-428C-B339-A9883501F19C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5C6F309-A1A2-46F0-A57B-68684D972651}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="56d601e6-bef3-45c8-b6dc-25c3b07e1d58"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated battery meter and colorization
</commit_message>
<xml_diff>
--- a/CCP Trade Tree Analysis.xlsx
+++ b/CCP Trade Tree Analysis.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuitenbr/Desktop/lunarspark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78AF22F-0694-904F-A8FD-08FF762A3F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF992F0-2944-C046-85CA-08A15B026590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{0D0644B8-F9A6-4A61-A91E-2BD3522A7E9F}"/>
+    <workbookView xWindow="0" yWindow="4500" windowWidth="30660" windowHeight="17900" activeTab="4" xr2:uid="{0D0644B8-F9A6-4A61-A91E-2BD3522A7E9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Laser Count Analysis" sheetId="4" r:id="rId1"/>
     <sheet name="Spacecraft Sizing" sheetId="5" r:id="rId2"/>
     <sheet name="Fleet cost analysis" sheetId="2" r:id="rId3"/>
     <sheet name="SE analysis" sheetId="1" r:id="rId4"/>
-    <sheet name="math" sheetId="3" r:id="rId5"/>
+    <sheet name="Pointing Eff" sheetId="6" r:id="rId5"/>
+    <sheet name="math" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="174">
   <si>
     <t>solar array size</t>
   </si>
@@ -514,6 +515,96 @@
   </si>
   <si>
     <t>Laser Panel eff</t>
+  </si>
+  <si>
+    <t>minimum elevation</t>
+  </si>
+  <si>
+    <t>maximum elevation</t>
+  </si>
+  <si>
+    <t>ideal case (flyover)</t>
+  </si>
+  <si>
+    <t>worst case (perpendicular flight)</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>moon radius</t>
+  </si>
+  <si>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>elevation</t>
+  </si>
+  <si>
+    <t>orbit altitude</t>
+  </si>
+  <si>
+    <t>nadir</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <r>
+      <t>𝜋</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FF232629"/>
+        <rFont val="STIXGeneral-Regular"/>
+      </rPr>
+      <t>∗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FF232629"/>
+        <rFont val="STIXGeneral-Italic"/>
+      </rPr>
+      <t>𝑟</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF232629"/>
+        <rFont val="STIXGeneral-Regular"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FF232629"/>
+        <rFont val="STIXGeneral-Regular"/>
+      </rPr>
+      <t>∗cos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FF232629"/>
+        <rFont val="STIXGeneral-Italic"/>
+      </rPr>
+      <t>𝜃</t>
+    </r>
+  </si>
+  <si>
+    <t>receiver diameter</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>effective area</t>
+  </si>
+  <si>
+    <t>receiver area</t>
   </si>
 </sst>
 </file>
@@ -524,7 +615,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -580,6 +671,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF232629"/>
+      <name val="STIXGeneral-Italic"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF232629"/>
+      <name val="STIXGeneral-Regular"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF232629"/>
+      <name val="STIXGeneral-Regular"/>
     </font>
   </fonts>
   <fills count="7">
@@ -740,7 +846,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -824,14 +930,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5896,6 +6007,187 @@
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>82066</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>728980</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>27939</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B92A9BF-5D26-6FAA-C4B0-7EC3F2F98CEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6197600" y="2012466"/>
+          <a:ext cx="2344420" cy="718033"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>75286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F7D2D51-F994-6966-9DD4-F0632CC6D59E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6167120" y="3312160"/>
+          <a:ext cx="7772400" cy="4078326"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>175602</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>424180</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>2539</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7BABDD4-1634-BC7E-0556-D50526DFF7B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8727440" y="1526882"/>
+          <a:ext cx="1978660" cy="1371257"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>81280</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>186112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DFD0C39-5A84-4BC2-AA67-E06FC5A1B9F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8717280" y="2888672"/>
+          <a:ext cx="2677160" cy="365067"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
@@ -6234,7 +6526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74459735-DBDE-7D4D-BD04-2A4022804EEC}">
   <dimension ref="A1:BR24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="AL34" sqref="AL34"/>
     </sheetView>
   </sheetViews>
@@ -6258,12 +6550,12 @@
       <c r="D1" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="50" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="46">
         <v>1300</v>
       </c>
@@ -6296,12 +6588,12 @@
       <c r="D2" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="46">
         <v>250</v>
       </c>
@@ -6333,12 +6625,12 @@
         <v>87</v>
       </c>
       <c r="E3" s="28"/>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="46">
         <v>61</v>
       </c>
@@ -6370,12 +6662,12 @@
         <v>89</v>
       </c>
       <c r="E4" s="25"/>
-      <c r="G4" s="48" t="s">
+      <c r="G4" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
       <c r="K4" s="46">
         <v>6</v>
       </c>
@@ -6894,202 +7186,202 @@
       <c r="D10" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="49">
+      <c r="E10" s="47">
         <v>0.85</v>
       </c>
-      <c r="F10" s="49">
+      <c r="F10" s="47">
         <v>0.85</v>
       </c>
-      <c r="G10" s="50">
+      <c r="G10" s="48">
         <v>0.85</v>
       </c>
-      <c r="H10" s="49">
+      <c r="H10" s="47">
         <v>0.85</v>
       </c>
-      <c r="I10" s="49">
+      <c r="I10" s="47">
         <v>0.85</v>
       </c>
-      <c r="J10" s="49">
+      <c r="J10" s="47">
         <v>0.85</v>
       </c>
-      <c r="K10" s="49">
+      <c r="K10" s="47">
         <v>0.85</v>
       </c>
-      <c r="L10" s="49">
+      <c r="L10" s="47">
         <v>0.85</v>
       </c>
-      <c r="M10" s="49">
+      <c r="M10" s="47">
         <v>0.85</v>
       </c>
-      <c r="N10" s="49">
+      <c r="N10" s="47">
         <v>0.85</v>
       </c>
-      <c r="O10" s="49">
+      <c r="O10" s="47">
         <v>0.85</v>
       </c>
-      <c r="P10" s="49">
+      <c r="P10" s="47">
         <v>0.85</v>
       </c>
-      <c r="Q10" s="49">
+      <c r="Q10" s="47">
         <v>0.85</v>
       </c>
-      <c r="R10" s="49">
+      <c r="R10" s="47">
         <v>0.85</v>
       </c>
-      <c r="S10" s="49">
+      <c r="S10" s="47">
         <v>0.85</v>
       </c>
-      <c r="T10" s="49">
+      <c r="T10" s="47">
         <v>0.85</v>
       </c>
-      <c r="U10" s="49">
+      <c r="U10" s="47">
         <v>0.85</v>
       </c>
-      <c r="V10" s="49">
+      <c r="V10" s="47">
         <v>0.85</v>
       </c>
-      <c r="W10" s="49">
+      <c r="W10" s="47">
         <v>0.85</v>
       </c>
-      <c r="X10" s="49">
+      <c r="X10" s="47">
         <v>0.85</v>
       </c>
-      <c r="Y10" s="49">
+      <c r="Y10" s="47">
         <v>0.85</v>
       </c>
-      <c r="Z10" s="49">
+      <c r="Z10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AA10" s="49">
+      <c r="AA10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AB10" s="50">
+      <c r="AB10" s="48">
         <v>0.85</v>
       </c>
-      <c r="AC10" s="49">
+      <c r="AC10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AD10" s="49">
+      <c r="AD10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AE10" s="49">
+      <c r="AE10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AF10" s="49">
+      <c r="AF10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AG10" s="49">
+      <c r="AG10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AH10" s="49">
+      <c r="AH10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AI10" s="49">
+      <c r="AI10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AJ10" s="49">
+      <c r="AJ10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AK10" s="49">
+      <c r="AK10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AL10" s="49">
+      <c r="AL10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AM10" s="49">
+      <c r="AM10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AN10" s="49">
+      <c r="AN10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AO10" s="49">
+      <c r="AO10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AP10" s="49">
+      <c r="AP10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AQ10" s="49">
+      <c r="AQ10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AR10" s="49">
+      <c r="AR10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AS10" s="49">
+      <c r="AS10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AT10" s="49">
+      <c r="AT10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AU10" s="49">
+      <c r="AU10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AV10" s="49">
+      <c r="AV10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AW10" s="49">
+      <c r="AW10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AX10" s="49">
+      <c r="AX10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AY10" s="49">
+      <c r="AY10" s="47">
         <v>0.85</v>
       </c>
-      <c r="AZ10" s="49">
+      <c r="AZ10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BA10" s="49">
+      <c r="BA10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BB10" s="49">
+      <c r="BB10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BC10" s="49">
+      <c r="BC10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BD10" s="49">
+      <c r="BD10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BE10" s="49">
+      <c r="BE10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BF10" s="49">
+      <c r="BF10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BG10" s="49">
+      <c r="BG10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BH10" s="49">
+      <c r="BH10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BI10" s="49">
+      <c r="BI10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BJ10" s="49">
+      <c r="BJ10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BK10" s="49">
+      <c r="BK10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BL10" s="49">
+      <c r="BL10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BM10" s="49">
+      <c r="BM10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BN10" s="49">
+      <c r="BN10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BO10" s="49">
+      <c r="BO10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BP10" s="49">
+      <c r="BP10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BQ10" s="49">
+      <c r="BQ10" s="47">
         <v>0.85</v>
       </c>
-      <c r="BR10" s="49">
+      <c r="BR10" s="47">
         <v>0.85</v>
       </c>
     </row>
@@ -7097,202 +7389,202 @@
       <c r="D11" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="E11" s="49">
+      <c r="E11" s="47">
         <v>0.4</v>
       </c>
-      <c r="F11" s="49">
+      <c r="F11" s="47">
         <v>0.4</v>
       </c>
-      <c r="G11" s="50">
+      <c r="G11" s="48">
         <v>0.4</v>
       </c>
-      <c r="H11" s="49">
+      <c r="H11" s="47">
         <v>0.4</v>
       </c>
-      <c r="I11" s="49">
+      <c r="I11" s="47">
         <v>0.4</v>
       </c>
-      <c r="J11" s="49">
+      <c r="J11" s="47">
         <v>0.4</v>
       </c>
-      <c r="K11" s="49">
+      <c r="K11" s="47">
         <v>0.4</v>
       </c>
-      <c r="L11" s="49">
+      <c r="L11" s="47">
         <v>0.4</v>
       </c>
-      <c r="M11" s="49">
+      <c r="M11" s="47">
         <v>0.4</v>
       </c>
-      <c r="N11" s="49">
+      <c r="N11" s="47">
         <v>0.4</v>
       </c>
-      <c r="O11" s="49">
+      <c r="O11" s="47">
         <v>0.4</v>
       </c>
-      <c r="P11" s="49">
+      <c r="P11" s="47">
         <v>0.4</v>
       </c>
-      <c r="Q11" s="49">
+      <c r="Q11" s="47">
         <v>0.4</v>
       </c>
-      <c r="R11" s="49">
+      <c r="R11" s="47">
         <v>0.4</v>
       </c>
-      <c r="S11" s="49">
+      <c r="S11" s="47">
         <v>0.4</v>
       </c>
-      <c r="T11" s="49">
+      <c r="T11" s="47">
         <v>0.4</v>
       </c>
-      <c r="U11" s="49">
+      <c r="U11" s="47">
         <v>0.4</v>
       </c>
-      <c r="V11" s="49">
+      <c r="V11" s="47">
         <v>0.4</v>
       </c>
-      <c r="W11" s="49">
+      <c r="W11" s="47">
         <v>0.4</v>
       </c>
-      <c r="X11" s="49">
+      <c r="X11" s="47">
         <v>0.4</v>
       </c>
-      <c r="Y11" s="49">
+      <c r="Y11" s="47">
         <v>0.4</v>
       </c>
-      <c r="Z11" s="49">
+      <c r="Z11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AA11" s="49">
+      <c r="AA11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AB11" s="50">
+      <c r="AB11" s="48">
         <v>0.4</v>
       </c>
-      <c r="AC11" s="49">
+      <c r="AC11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AD11" s="49">
+      <c r="AD11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AE11" s="49">
+      <c r="AE11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AF11" s="49">
+      <c r="AF11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AG11" s="49">
+      <c r="AG11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AH11" s="49">
+      <c r="AH11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AI11" s="49">
+      <c r="AI11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AJ11" s="49">
+      <c r="AJ11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AK11" s="49">
+      <c r="AK11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AL11" s="49">
+      <c r="AL11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AM11" s="49">
+      <c r="AM11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AN11" s="49">
+      <c r="AN11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AO11" s="49">
+      <c r="AO11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AP11" s="49">
+      <c r="AP11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AQ11" s="49">
+      <c r="AQ11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AR11" s="49">
+      <c r="AR11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AS11" s="49">
+      <c r="AS11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AT11" s="49">
+      <c r="AT11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AU11" s="49">
+      <c r="AU11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AV11" s="49">
+      <c r="AV11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AW11" s="49">
+      <c r="AW11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AX11" s="49">
+      <c r="AX11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AY11" s="49">
+      <c r="AY11" s="47">
         <v>0.4</v>
       </c>
-      <c r="AZ11" s="49">
+      <c r="AZ11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BA11" s="49">
+      <c r="BA11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BB11" s="49">
+      <c r="BB11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BC11" s="49">
+      <c r="BC11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BD11" s="49">
+      <c r="BD11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BE11" s="49">
+      <c r="BE11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BF11" s="49">
+      <c r="BF11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BG11" s="49">
+      <c r="BG11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BH11" s="49">
+      <c r="BH11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BI11" s="49">
+      <c r="BI11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BJ11" s="49">
+      <c r="BJ11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BK11" s="49">
+      <c r="BK11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BL11" s="49">
+      <c r="BL11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BM11" s="49">
+      <c r="BM11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BN11" s="49">
+      <c r="BN11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BO11" s="49">
+      <c r="BO11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BP11" s="49">
+      <c r="BP11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BQ11" s="49">
+      <c r="BQ11" s="47">
         <v>0.4</v>
       </c>
-      <c r="BR11" s="49">
+      <c r="BR11" s="47">
         <v>0.4</v>
       </c>
     </row>
@@ -7300,202 +7592,202 @@
       <c r="D12" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="E12" s="49">
+      <c r="E12" s="47">
         <v>0.85</v>
       </c>
-      <c r="F12" s="49">
+      <c r="F12" s="47">
         <v>0.85</v>
       </c>
-      <c r="G12" s="50">
+      <c r="G12" s="48">
         <v>0.85</v>
       </c>
-      <c r="H12" s="49">
+      <c r="H12" s="47">
         <v>0.85</v>
       </c>
-      <c r="I12" s="49">
+      <c r="I12" s="47">
         <v>0.85</v>
       </c>
-      <c r="J12" s="49">
+      <c r="J12" s="47">
         <v>0.85</v>
       </c>
-      <c r="K12" s="49">
+      <c r="K12" s="47">
         <v>0.85</v>
       </c>
-      <c r="L12" s="49">
+      <c r="L12" s="47">
         <v>0.85</v>
       </c>
-      <c r="M12" s="49">
+      <c r="M12" s="47">
         <v>0.85</v>
       </c>
-      <c r="N12" s="49">
+      <c r="N12" s="47">
         <v>0.85</v>
       </c>
-      <c r="O12" s="49">
+      <c r="O12" s="47">
         <v>0.85</v>
       </c>
-      <c r="P12" s="49">
+      <c r="P12" s="47">
         <v>0.85</v>
       </c>
-      <c r="Q12" s="49">
+      <c r="Q12" s="47">
         <v>0.85</v>
       </c>
-      <c r="R12" s="49">
+      <c r="R12" s="47">
         <v>0.85</v>
       </c>
-      <c r="S12" s="49">
+      <c r="S12" s="47">
         <v>0.85</v>
       </c>
-      <c r="T12" s="49">
+      <c r="T12" s="47">
         <v>0.85</v>
       </c>
-      <c r="U12" s="49">
+      <c r="U12" s="47">
         <v>0.85</v>
       </c>
-      <c r="V12" s="49">
+      <c r="V12" s="47">
         <v>0.85</v>
       </c>
-      <c r="W12" s="49">
+      <c r="W12" s="47">
         <v>0.85</v>
       </c>
-      <c r="X12" s="49">
+      <c r="X12" s="47">
         <v>0.85</v>
       </c>
-      <c r="Y12" s="49">
+      <c r="Y12" s="47">
         <v>0.85</v>
       </c>
-      <c r="Z12" s="49">
+      <c r="Z12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AA12" s="49">
+      <c r="AA12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AB12" s="49">
+      <c r="AB12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AC12" s="49">
+      <c r="AC12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AD12" s="49">
+      <c r="AD12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AE12" s="49">
+      <c r="AE12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AF12" s="49">
+      <c r="AF12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AG12" s="49">
+      <c r="AG12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AH12" s="49">
+      <c r="AH12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AI12" s="49">
+      <c r="AI12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AJ12" s="49">
+      <c r="AJ12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AK12" s="49">
+      <c r="AK12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AL12" s="49">
+      <c r="AL12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AM12" s="49">
+      <c r="AM12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AN12" s="49">
+      <c r="AN12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AO12" s="49">
+      <c r="AO12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AP12" s="49">
+      <c r="AP12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AQ12" s="49">
+      <c r="AQ12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AR12" s="49">
+      <c r="AR12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AS12" s="49">
+      <c r="AS12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AT12" s="49">
+      <c r="AT12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AU12" s="49">
+      <c r="AU12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AV12" s="49">
+      <c r="AV12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AW12" s="49">
+      <c r="AW12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AX12" s="49">
+      <c r="AX12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AY12" s="49">
+      <c r="AY12" s="47">
         <v>0.85</v>
       </c>
-      <c r="AZ12" s="49">
+      <c r="AZ12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BA12" s="49">
+      <c r="BA12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BB12" s="49">
+      <c r="BB12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BC12" s="49">
+      <c r="BC12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BD12" s="49">
+      <c r="BD12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BE12" s="49">
+      <c r="BE12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BF12" s="49">
+      <c r="BF12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BG12" s="49">
+      <c r="BG12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BH12" s="49">
+      <c r="BH12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BI12" s="49">
+      <c r="BI12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BJ12" s="49">
+      <c r="BJ12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BK12" s="49">
+      <c r="BK12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BL12" s="49">
+      <c r="BL12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BM12" s="49">
+      <c r="BM12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BN12" s="49">
+      <c r="BN12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BO12" s="49">
+      <c r="BO12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BP12" s="49">
+      <c r="BP12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BQ12" s="49">
+      <c r="BQ12" s="47">
         <v>0.85</v>
       </c>
-      <c r="BR12" s="49">
+      <c r="BR12" s="47">
         <v>0.85</v>
       </c>
     </row>
@@ -8853,7 +9145,7 @@
       <c r="AB19" s="40"/>
     </row>
     <row r="20" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A20" s="47"/>
+      <c r="A20" s="49"/>
       <c r="D20" s="26" t="s">
         <v>96</v>
       </c>
@@ -9123,7 +9415,7 @@
       </c>
     </row>
     <row r="21" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A21" s="47"/>
+      <c r="A21" s="49"/>
       <c r="D21" s="26" t="s">
         <v>97</v>
       </c>
@@ -9393,7 +9685,7 @@
       </c>
     </row>
     <row r="22" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A22" s="47"/>
+      <c r="A22" s="49"/>
       <c r="D22" s="26" t="s">
         <v>98</v>
       </c>
@@ -10229,12 +10521,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="23">
         <f>'Laser Count Analysis'!K2</f>
         <v>250</v>
@@ -10244,12 +10536,12 @@
       </c>
     </row>
     <row r="2" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
       <c r="F2" s="23">
         <f>'Laser Count Analysis'!K3</f>
         <v>61</v>
@@ -10259,12 +10551,12 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
       <c r="F3" s="23">
         <f>'Laser Count Analysis'!K4</f>
         <v>6</v>
@@ -10371,40 +10663,40 @@
       <c r="B7" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="47">
         <v>0.15</v>
       </c>
-      <c r="D7" s="49">
+      <c r="D7" s="47">
         <v>0.15</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="47">
         <v>0.15</v>
       </c>
-      <c r="F7" s="49">
+      <c r="F7" s="47">
         <v>0.15</v>
       </c>
-      <c r="G7" s="49">
+      <c r="G7" s="47">
         <v>0.15</v>
       </c>
-      <c r="H7" s="49">
+      <c r="H7" s="47">
         <v>0.15</v>
       </c>
-      <c r="I7" s="49">
+      <c r="I7" s="47">
         <v>0.15</v>
       </c>
-      <c r="J7" s="49">
+      <c r="J7" s="47">
         <v>0.15</v>
       </c>
-      <c r="K7" s="49">
+      <c r="K7" s="47">
         <v>0.15</v>
       </c>
-      <c r="L7" s="49">
+      <c r="L7" s="47">
         <v>0.15</v>
       </c>
-      <c r="M7" s="49">
+      <c r="M7" s="47">
         <v>0.15</v>
       </c>
-      <c r="N7" s="49">
+      <c r="N7" s="47">
         <v>0.15</v>
       </c>
       <c r="P7" t="s">
@@ -10574,40 +10866,40 @@
       <c r="B11" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="C11" s="49">
+      <c r="C11" s="47">
         <v>0.85</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D11" s="47">
         <v>0.85</v>
       </c>
-      <c r="E11" s="49">
+      <c r="E11" s="47">
         <v>0.85</v>
       </c>
-      <c r="F11" s="49">
+      <c r="F11" s="47">
         <v>0.85</v>
       </c>
-      <c r="G11" s="49">
+      <c r="G11" s="47">
         <v>0.85</v>
       </c>
-      <c r="H11" s="49">
+      <c r="H11" s="47">
         <v>0.85</v>
       </c>
-      <c r="I11" s="49">
+      <c r="I11" s="47">
         <v>0.85</v>
       </c>
-      <c r="J11" s="49">
+      <c r="J11" s="47">
         <v>0.85</v>
       </c>
-      <c r="K11" s="49">
+      <c r="K11" s="47">
         <v>0.85</v>
       </c>
-      <c r="L11" s="49">
+      <c r="L11" s="47">
         <v>0.85</v>
       </c>
-      <c r="M11" s="49">
+      <c r="M11" s="47">
         <v>0.85</v>
       </c>
-      <c r="N11" s="49">
+      <c r="N11" s="47">
         <v>0.85</v>
       </c>
     </row>
@@ -10815,40 +11107,40 @@
       <c r="B17" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="C17" s="49">
+      <c r="C17" s="47">
         <v>0.75</v>
       </c>
-      <c r="D17" s="49">
+      <c r="D17" s="47">
         <v>0.75</v>
       </c>
-      <c r="E17" s="49">
+      <c r="E17" s="47">
         <v>0.75</v>
       </c>
-      <c r="F17" s="49">
+      <c r="F17" s="47">
         <v>0.75</v>
       </c>
-      <c r="G17" s="49">
+      <c r="G17" s="47">
         <v>0.75</v>
       </c>
-      <c r="H17" s="49">
+      <c r="H17" s="47">
         <v>0.75</v>
       </c>
-      <c r="I17" s="49">
+      <c r="I17" s="47">
         <v>0.75</v>
       </c>
-      <c r="J17" s="49">
+      <c r="J17" s="47">
         <v>0.75</v>
       </c>
-      <c r="K17" s="49">
+      <c r="K17" s="47">
         <v>0.75</v>
       </c>
-      <c r="L17" s="49">
+      <c r="L17" s="47">
         <v>0.75</v>
       </c>
-      <c r="M17" s="49">
+      <c r="M17" s="47">
         <v>0.75</v>
       </c>
-      <c r="N17" s="49">
+      <c r="N17" s="47">
         <v>0.75</v>
       </c>
     </row>
@@ -10950,40 +11242,40 @@
       <c r="B20" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C20" s="49">
+      <c r="C20" s="47">
         <v>0.4</v>
       </c>
-      <c r="D20" s="49">
+      <c r="D20" s="47">
         <v>0.4</v>
       </c>
-      <c r="E20" s="49">
+      <c r="E20" s="47">
         <v>0.4</v>
       </c>
-      <c r="F20" s="49">
+      <c r="F20" s="47">
         <v>0.4</v>
       </c>
-      <c r="G20" s="49">
+      <c r="G20" s="47">
         <v>0.4</v>
       </c>
-      <c r="H20" s="49">
+      <c r="H20" s="47">
         <v>0.4</v>
       </c>
-      <c r="I20" s="49">
+      <c r="I20" s="47">
         <v>0.4</v>
       </c>
-      <c r="J20" s="49">
+      <c r="J20" s="47">
         <v>0.4</v>
       </c>
-      <c r="K20" s="49">
+      <c r="K20" s="47">
         <v>0.4</v>
       </c>
-      <c r="L20" s="49">
+      <c r="L20" s="47">
         <v>0.4</v>
       </c>
-      <c r="M20" s="49">
+      <c r="M20" s="47">
         <v>0.4</v>
       </c>
-      <c r="N20" s="49">
+      <c r="N20" s="47">
         <v>0.4</v>
       </c>
     </row>
@@ -14157,6 +14449,373 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1EB7CC8-2E43-AD42-9797-36D0C73BF74C}">
+  <dimension ref="C2:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C2" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2">
+        <v>1373</v>
+      </c>
+      <c r="E2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2">
+        <v>1373</v>
+      </c>
+      <c r="G2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3">
+        <v>402</v>
+      </c>
+      <c r="E3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3">
+        <v>1300</v>
+      </c>
+      <c r="G3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="26"/>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C5" s="26" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7">
+        <v>90</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7">
+        <v>90</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="26"/>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C9" s="26" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C10" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C11" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="D11">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11">
+        <v>67</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C13" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" s="1">
+        <f>RADIANS(D14)</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="1">
+        <f>RADIANS(F14)</f>
+        <v>1.1693705988362009</v>
+      </c>
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C14" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14" s="5">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="5">
+        <v>67</v>
+      </c>
+      <c r="G14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C15" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" s="1">
+        <f>ASIN((D2/(D2+D3)))</f>
+        <v>0.88437830828608255</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="1">
+        <f>ASIN((F2/(F2+F3)))</f>
+        <v>0.53943938812170644</v>
+      </c>
+      <c r="G15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C16" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" s="2">
+        <f>DEGREES(D15)</f>
+        <v>50.671144557712132</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" ref="F16" si="0">DEGREES(F15)</f>
+        <v>30.907600242493331</v>
+      </c>
+      <c r="G16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C17" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" s="2">
+        <f>ASIN(COS(D13)*SIN(D15))</f>
+        <v>0.57873101123750248</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="2">
+        <f>ASIN(COS(F13)*SIN(F15))</f>
+        <v>0.20207345359416248</v>
+      </c>
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C18" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="D18" s="2">
+        <f>DEGREES(D17)</f>
+        <v>33.15884441724711</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="2">
+        <f>DEGREES(F17)</f>
+        <v>11.577956042578206</v>
+      </c>
+      <c r="G18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C19" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19" s="2">
+        <f>RADIANS(90-D14-D18)</f>
+        <v>0.2066671521599458</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="2">
+        <f>RADIANS(90-F14-F18)</f>
+        <v>0.19935227436453332</v>
+      </c>
+      <c r="G19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C20" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="2">
+        <f>DEGREES(D19)</f>
+        <v>11.84115558275289</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="2">
+        <f>DEGREES(F19)</f>
+        <v>11.422043957421794</v>
+      </c>
+      <c r="G20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C21" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="3">
+        <f>D2*(SIN(D19)/SIN(D17))</f>
+        <v>515.09679653762919</v>
+      </c>
+      <c r="E21" t="s">
+        <v>152</v>
+      </c>
+      <c r="F21" s="3">
+        <f>F2*(SIN(F19)/SIN(F17))</f>
+        <v>1354.7580749435103</v>
+      </c>
+      <c r="G21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C24" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24" s="5">
+        <v>50</v>
+      </c>
+      <c r="E24" t="s">
+        <v>171</v>
+      </c>
+      <c r="F24" s="5">
+        <v>50</v>
+      </c>
+      <c r="G24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C25" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25" s="53">
+        <f>PI()*(D24/100)^2</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="53">
+        <f>PI()*(F24/100)^2</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" ht="29" x14ac:dyDescent="0.4">
+      <c r="C26" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="52">
+        <f>PI()*(D24/100)^2*COS(RADIANS(90)-D13)</f>
+        <v>0.55536036726979576</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="52">
+        <f>PI()*(F24/100)^2*COS(RADIANS(90)-F13)</f>
+        <v>0.7229628212999839</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" s="51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E790B1-52D8-A842-8268-804FFB128667}">
   <dimension ref="A2:Q56"/>
   <sheetViews>
@@ -15516,25 +16175,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56d601e6-bef3-45c8-b6dc-25c3b07e1d58">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100870398E7EAE9954ABE6BFB497661637E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3786cb5e95af3a90c677764e8014d423">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56d601e6-bef3-45c8-b6dc-25c3b07e1d58" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="adb27d47ef9772e2cb84c18b7530cab2" ns2:_="">
     <xsd:import namespace="56d601e6-bef3-45c8-b6dc-25c3b07e1d58"/>
@@ -15720,10 +16360,39 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56d601e6-bef3-45c8-b6dc-25c3b07e1d58">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5C6F309-A1A2-46F0-A57B-68684D972651}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD5649D0-F6D4-456F-915F-B334A3145553}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="56d601e6-bef3-45c8-b6dc-25c3b07e1d58"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15739,19 +16408,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD5649D0-F6D4-456F-915F-B334A3145553}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5C6F309-A1A2-46F0-A57B-68684D972651}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="56d601e6-bef3-45c8-b6dc-25c3b07e1d58"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated excel with pointing data
</commit_message>
<xml_diff>
--- a/CCP Trade Tree Analysis.xlsx
+++ b/CCP Trade Tree Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuitenbr/Desktop/lunarspark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF992F0-2944-C046-85CA-08A15B026590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F55901B-EE03-B441-A2EF-C421BFB4BBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4500" windowWidth="30660" windowHeight="17900" activeTab="4" xr2:uid="{0D0644B8-F9A6-4A61-A91E-2BD3522A7E9F}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Spacecraft Sizing" sheetId="5" r:id="rId2"/>
     <sheet name="Fleet cost analysis" sheetId="2" r:id="rId3"/>
     <sheet name="SE analysis" sheetId="1" r:id="rId4"/>
-    <sheet name="Pointing Eff" sheetId="6" r:id="rId5"/>
+    <sheet name="Pointing Eff Acc" sheetId="6" r:id="rId5"/>
     <sheet name="math" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="192">
   <si>
     <t>solar array size</t>
   </si>
@@ -548,6 +548,18 @@
   </si>
   <si>
     <t>lambda</t>
+  </si>
+  <si>
+    <t>receiver diameter</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>effective area</t>
+  </si>
+  <si>
+    <t>receiver area</t>
   </si>
   <si>
     <r>
@@ -555,7 +567,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="17"/>
+        <sz val="14"/>
         <color rgb="FF232629"/>
         <rFont val="STIXGeneral-Regular"/>
       </rPr>
@@ -563,7 +575,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="17"/>
+        <sz val="14"/>
         <color rgb="FF232629"/>
         <rFont val="STIXGeneral-Italic"/>
       </rPr>
@@ -571,23 +583,15 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="14"/>
         <color rgb="FF232629"/>
         <rFont val="STIXGeneral-Regular"/>
       </rPr>
-      <t>2</t>
+      <t>2∗cos</t>
     </r>
     <r>
       <rPr>
-        <sz val="17"/>
-        <color rgb="FF232629"/>
-        <rFont val="STIXGeneral-Regular"/>
-      </rPr>
-      <t>∗cos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="17"/>
+        <sz val="14"/>
         <color rgb="FF232629"/>
         <rFont val="STIXGeneral-Italic"/>
       </rPr>
@@ -595,16 +599,58 @@
     </r>
   </si>
   <si>
-    <t>receiver diameter</t>
-  </si>
-  <si>
-    <t>cm</t>
-  </si>
-  <si>
-    <t>effective area</t>
-  </si>
-  <si>
-    <t>receiver area</t>
+    <t>𝜃=90-elev</t>
+  </si>
+  <si>
+    <t>error tolerance</t>
+  </si>
+  <si>
+    <t>(beam dia - rec diam) / 2</t>
+  </si>
+  <si>
+    <t>pointing accuracy tolerance</t>
+  </si>
+  <si>
+    <t>urad</t>
+  </si>
+  <si>
+    <t>https://www.mdpi.com/2413-4155/3/1/4#:~:text=hundred%20kilometers%20away.-,3.2.2,-.%20Acquisition%2C%20Tracking%2C%20and</t>
+  </si>
+  <si>
+    <t>atan(error tol/range)</t>
+  </si>
+  <si>
+    <t>ideal alignment</t>
+  </si>
+  <si>
+    <t>misaligned by (beam dia - rcv dia)/2</t>
+  </si>
+  <si>
+    <t>initial beam diameter</t>
+  </si>
+  <si>
+    <t>beam diameter at rcvr</t>
+  </si>
+  <si>
+    <t>assume columnated?</t>
+  </si>
+  <si>
+    <t>eff rcvr area/beam area</t>
+  </si>
+  <si>
+    <t>beam area at rcvr</t>
+  </si>
+  <si>
+    <t>elevation adjusted eff</t>
+  </si>
+  <si>
+    <t>required pointing accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need to consider elevations greater than 30 deg to get 90%+ efficiency </t>
+  </si>
+  <si>
+    <t>this graph not accounted for in calculations</t>
   </si>
 </sst>
 </file>
@@ -615,7 +661,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,17 +719,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="17"/>
+      <sz val="14"/>
       <color rgb="FF232629"/>
       <name val="STIXGeneral-Italic"/>
     </font>
     <font>
-      <sz val="17"/>
-      <color rgb="FF232629"/>
-      <name val="STIXGeneral-Regular"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <sz val="14"/>
       <color rgb="FF232629"/>
       <name val="STIXGeneral-Regular"/>
     </font>
@@ -846,7 +887,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -938,11 +979,12 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6007,6 +6049,69 @@
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>172720</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Oval 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5992CF1C-AF6E-414E-B9AF-252A9066BF33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6350000" y="7223760"/>
+          <a:ext cx="812800" cy="751840"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>beam</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -6053,16 +6158,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>75286</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>144271</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6085,8 +6190,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6167120" y="3312160"/>
-          <a:ext cx="7772400" cy="4078326"/>
+          <a:off x="10891520" y="0"/>
+          <a:ext cx="5425440" cy="2846831"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6181,6 +6286,325 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>422174</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>162560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>721772</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>116840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30F2E088-4336-6984-5769-CAC3173FEC73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6589294" y="3830320"/>
+          <a:ext cx="5237358" cy="3134360"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>325120</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>10160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Oval 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44A7CC88-3E8E-8327-E82D-FC0C972B50BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6492240" y="7213600"/>
+          <a:ext cx="528320" cy="447040"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>rcv</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>20320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>802640</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>10160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Right Triangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08C56E4C-3F87-DC38-B6D4-408DF8E32180}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6725920" y="7477760"/>
+          <a:ext cx="2712720" cy="182880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rtTriangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>81280</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>71120</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Oval 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A4D2775-9DE5-F84E-8E0E-95C364A4D391}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5425440" y="7752080"/>
+          <a:ext cx="812800" cy="751840"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>beam</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>223520</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>751840</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Oval 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2020A48C-FAF3-0D43-A6A8-8B7271237CA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5567680" y="7904480"/>
+          <a:ext cx="528320" cy="447040"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>rcv</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -14450,10 +14874,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1EB7CC8-2E43-AD42-9797-36D0C73BF74C}">
-  <dimension ref="C2:H26"/>
+  <dimension ref="C2:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14588,14 +15012,14 @@
       </c>
       <c r="D13" s="1">
         <f>RADIANS(D14)</f>
-        <v>0.78539816339744828</v>
+        <v>0.52359877559829882</v>
       </c>
       <c r="E13" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="1">
         <f>RADIANS(F14)</f>
-        <v>1.1693705988362009</v>
+        <v>0.52359877559829882</v>
       </c>
       <c r="G13" t="s">
         <v>47</v>
@@ -14606,13 +15030,13 @@
         <v>165</v>
       </c>
       <c r="D14" s="5">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
         <v>46</v>
       </c>
       <c r="F14" s="5">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
         <v>46</v>
@@ -14656,121 +15080,127 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C17" s="26" t="s">
         <v>167</v>
       </c>
       <c r="D17" s="2">
         <f>ASIN(COS(D13)*SIN(D15))</f>
-        <v>0.57873101123750248</v>
+        <v>0.7340592020747656</v>
       </c>
       <c r="E17" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="2">
         <f>ASIN(COS(F13)*SIN(F15))</f>
-        <v>0.20207345359416248</v>
+        <v>0.46099374881500926</v>
       </c>
       <c r="G17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C18" s="26" t="s">
         <v>167</v>
       </c>
       <c r="D18" s="2">
         <f>DEGREES(D17)</f>
-        <v>33.15884441724711</v>
+        <v>42.058494191624909</v>
       </c>
       <c r="E18" t="s">
         <v>46</v>
       </c>
       <c r="F18" s="2">
         <f>DEGREES(F17)</f>
-        <v>11.577956042578206</v>
+        <v>26.412996189014027</v>
       </c>
       <c r="G18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C19" s="26" t="s">
         <v>168</v>
       </c>
       <c r="D19" s="2">
         <f>RADIANS(90-D14-D18)</f>
-        <v>0.2066671521599458</v>
+        <v>0.31313834912183214</v>
       </c>
       <c r="E19" t="s">
         <v>47</v>
       </c>
       <c r="F19" s="2">
         <f>RADIANS(90-F14-F18)</f>
-        <v>0.19935227436453332</v>
+        <v>0.58620380238158853</v>
       </c>
       <c r="G19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C20" s="26" t="s">
         <v>168</v>
       </c>
       <c r="D20" s="2">
         <f>DEGREES(D19)</f>
-        <v>11.84115558275289</v>
+        <v>17.941505808375091</v>
       </c>
       <c r="E20" t="s">
         <v>46</v>
       </c>
       <c r="F20" s="2">
         <f>DEGREES(F19)</f>
-        <v>11.422043957421794</v>
+        <v>33.587003810985976</v>
       </c>
       <c r="G20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C21" s="26" t="s">
         <v>162</v>
       </c>
       <c r="D21" s="3">
         <f>D2*(SIN(D19)/SIN(D17))</f>
-        <v>515.09679653762919</v>
+        <v>631.36882882933344</v>
       </c>
       <c r="E21" t="s">
         <v>152</v>
       </c>
       <c r="F21" s="3">
         <f>F2*(SIN(F19)/SIN(F17))</f>
-        <v>1354.7580749435103</v>
+        <v>1707.4678882558132</v>
       </c>
       <c r="G21" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="J23" s="32"/>
+    </row>
+    <row r="24" spans="3:19" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D24" s="5">
         <v>50</v>
       </c>
       <c r="E24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F24" s="5">
         <v>50</v>
       </c>
       <c r="G24" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C25" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D25" s="53">
         <f>PI()*(D24/100)^2</f>
@@ -14786,30 +15216,187 @@
       <c r="G25" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="3:8" ht="29" x14ac:dyDescent="0.4">
+      <c r="H25" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q25" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="R25" s="49"/>
+      <c r="S25" s="49"/>
+    </row>
+    <row r="26" spans="3:19" ht="25" x14ac:dyDescent="0.35">
       <c r="C26" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="D26" s="52">
+        <v>171</v>
+      </c>
+      <c r="D26" s="51">
         <f>PI()*(D24/100)^2*COS(RADIANS(90)-D13)</f>
-        <v>0.55536036726979576</v>
+        <v>0.39269908169872403</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="52">
+      <c r="F26" s="51">
         <f>PI()*(F24/100)^2*COS(RADIANS(90)-F13)</f>
-        <v>0.7229628212999839</v>
+        <v>0.39269908169872403</v>
       </c>
       <c r="G26" t="s">
         <v>1</v>
       </c>
-      <c r="H26" s="51" t="s">
-        <v>169</v>
+      <c r="H26" s="54" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C28" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D28" s="5">
+        <v>85</v>
+      </c>
+      <c r="E28" t="s">
+        <v>170</v>
+      </c>
+      <c r="F28" s="5">
+        <v>85</v>
+      </c>
+      <c r="G28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C29" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="D29" s="52">
+        <f>D28</f>
+        <v>85</v>
+      </c>
+      <c r="E29" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="F29" s="52">
+        <f>F28</f>
+        <v>85</v>
+      </c>
+      <c r="G29" t="s">
+        <v>170</v>
+      </c>
+      <c r="H29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C30" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="D30" s="53">
+        <f>2*PI()*(D29/100/2)^2</f>
+        <v>1.1349003461093126</v>
+      </c>
+      <c r="E30" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="53">
+        <f>2*PI()*(F29/100/2)^2</f>
+        <v>1.1349003461093126</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C32" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="D32">
+        <f>(D29-D24)/2</f>
+        <v>17.5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>170</v>
+      </c>
+      <c r="F32">
+        <f>(F29-F24)/2</f>
+        <v>17.5</v>
+      </c>
+      <c r="G32" t="s">
+        <v>170</v>
+      </c>
+      <c r="H32" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C34" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="D34" s="1">
+        <f>ATAN((D32/100)/(D21*1000))*10000000</f>
+        <v>2.7717554622466181</v>
+      </c>
+      <c r="E34" t="s">
+        <v>178</v>
+      </c>
+      <c r="F34" s="1">
+        <f>ATAN((F32/100)/(F21*1000))*10000000</f>
+        <v>1.0249094650837782</v>
+      </c>
+      <c r="G34" t="s">
+        <v>178</v>
+      </c>
+      <c r="H34" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C35" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="D35" s="1">
+        <f>D26/D30</f>
+        <v>0.34602076124567471</v>
+      </c>
+      <c r="F35" s="1">
+        <f>F26/F30</f>
+        <v>0.34602076124567471</v>
+      </c>
+      <c r="H35" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="M40" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="I41" t="s">
+        <v>175</v>
+      </c>
+      <c r="N41" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="L42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="K43" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="J45" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="Q25:S25"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added incidence ange efficiency to model
</commit_message>
<xml_diff>
--- a/CCP Trade Tree Analysis.xlsx
+++ b/CCP Trade Tree Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuitenbr/Desktop/lunarspark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F55901B-EE03-B441-A2EF-C421BFB4BBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E9B94D-A9FE-F740-A32B-6E4740B49948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4500" windowWidth="30660" windowHeight="17900" activeTab="4" xr2:uid="{0D0644B8-F9A6-4A61-A91E-2BD3522A7E9F}"/>
+    <workbookView xWindow="0" yWindow="1280" windowWidth="33800" windowHeight="21120" activeTab="4" xr2:uid="{0D0644B8-F9A6-4A61-A91E-2BD3522A7E9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Laser Count Analysis" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="194">
   <si>
     <t>solar array size</t>
   </si>
@@ -641,9 +641,6 @@
     <t>beam area at rcvr</t>
   </si>
   <si>
-    <t>elevation adjusted eff</t>
-  </si>
-  <si>
     <t>required pointing accuracy</t>
   </si>
   <si>
@@ -651,6 +648,15 @@
   </si>
   <si>
     <t>this graph not accounted for in calculations</t>
+  </si>
+  <si>
+    <t>laser panel eff (0 deg)</t>
+  </si>
+  <si>
+    <t>elevation + beam diameter adjustment</t>
+  </si>
+  <si>
+    <t>overall adjusted eff</t>
   </si>
 </sst>
 </file>
@@ -887,7 +893,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -985,6 +991,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3424,6 +3431,517 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Elevation</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Angle and Beam Diameter Eficiency</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pointing Eff Acc'!$C$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>elevation + beam diameter adjustment</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Pointing Eff Acc'!$F$14:$K$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pointing Eff Acc'!$F$36:$K$36</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.4704761275630185E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17677669529663689</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.21650635094610965</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24148145657226708</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24996192378909782</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-386A-B241-BDD5-A7F629071786}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pointing Eff Acc'!$C$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>overall adjusted eff</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Pointing Eff Acc'!$F$14:$K$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pointing Eff Acc'!$F$37:$K$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.5881904510252074E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9999999999999989E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0710678118654766E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.6602540378443865E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.659258262890684E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.998476951563913E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-386A-B241-BDD5-A7F629071786}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="366622191"/>
+        <c:axId val="366623839"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="366622191"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>elevaion angle (deg)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="366623839"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="366623839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="366622191"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3750,6 +4268,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5824,6 +6382,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6051,15 +7125,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>172720</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>132080</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6114,13 +7188,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>82066</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>728980</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>27939</xdr:rowOff>
@@ -6158,13 +7232,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>274320</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>144271</xdr:rowOff>
@@ -6202,13 +7276,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>91440</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>175602</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>424180</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>2539</xdr:rowOff>
@@ -6246,13 +7320,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>81280</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>186112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>165099</xdr:rowOff>
@@ -6290,13 +7364,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>422174</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>162560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>721772</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>116840</xdr:rowOff>
@@ -6351,15 +7425,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>325120</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>142240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>10160</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6417,15 +7491,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>20320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>802640</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>10160</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6480,15 +7554,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>81280</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>71120</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>81280</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6543,15 +7617,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>223520</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>751840</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6605,6 +7679,42 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>20320</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>10160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>421640</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{364B206B-7853-BB0A-16AE-F81854932B69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -14874,21 +15984,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1EB7CC8-2E43-AD42-9797-36D0C73BF74C}">
-  <dimension ref="C2:S45"/>
+  <dimension ref="C2:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" customWidth="1"/>
-    <col min="7" max="7" width="5.1640625" customWidth="1"/>
+    <col min="6" max="11" width="8.1640625" customWidth="1"/>
+    <col min="12" max="12" width="5.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C2" s="26" t="s">
         <v>163</v>
       </c>
@@ -14901,36 +16011,66 @@
       <c r="F2">
         <v>1373</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>1373</v>
+      </c>
+      <c r="H2">
+        <v>1373</v>
+      </c>
+      <c r="I2">
+        <v>1373</v>
+      </c>
+      <c r="J2">
+        <v>1373</v>
+      </c>
+      <c r="K2">
+        <v>1373</v>
+      </c>
+      <c r="L2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C3" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>402</v>
       </c>
       <c r="E3" t="s">
         <v>152</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="5">
         <v>1300</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="5">
+        <v>1300</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1300</v>
+      </c>
+      <c r="I3" s="5">
+        <v>1300</v>
+      </c>
+      <c r="J3" s="5">
+        <v>1300</v>
+      </c>
+      <c r="K3" s="5">
+        <v>1300</v>
+      </c>
+      <c r="L3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C4" s="26"/>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C5" s="26" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C6" s="26" t="s">
         <v>158</v>
       </c>
@@ -14943,11 +16083,26 @@
       <c r="F6">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>12</v>
+      </c>
+      <c r="K6">
+        <v>12</v>
+      </c>
+      <c r="L6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C7" s="26" t="s">
         <v>159</v>
       </c>
@@ -14960,19 +16115,34 @@
       <c r="F7">
         <v>90</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7">
+        <v>90</v>
+      </c>
+      <c r="H7">
+        <v>90</v>
+      </c>
+      <c r="I7">
+        <v>90</v>
+      </c>
+      <c r="J7">
+        <v>90</v>
+      </c>
+      <c r="K7">
+        <v>90</v>
+      </c>
+      <c r="L7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C8" s="26"/>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C9" s="26" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C10" s="26" t="s">
         <v>158</v>
       </c>
@@ -14985,11 +16155,26 @@
       <c r="F10">
         <v>12</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <v>12</v>
+      </c>
+      <c r="I10">
+        <v>12</v>
+      </c>
+      <c r="J10">
+        <v>12</v>
+      </c>
+      <c r="K10">
+        <v>12</v>
+      </c>
+      <c r="L10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C11" s="26" t="s">
         <v>159</v>
       </c>
@@ -15002,47 +16187,97 @@
       <c r="F11">
         <v>67</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11">
+        <v>67</v>
+      </c>
+      <c r="H11">
+        <v>67</v>
+      </c>
+      <c r="I11">
+        <v>67</v>
+      </c>
+      <c r="J11">
+        <v>67</v>
+      </c>
+      <c r="K11">
+        <v>67</v>
+      </c>
+      <c r="L11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C13" s="26" t="s">
         <v>165</v>
       </c>
       <c r="D13" s="1">
         <f>RADIANS(D14)</f>
-        <v>0.52359877559829882</v>
+        <v>1.5533430342749532</v>
       </c>
       <c r="E13" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="1">
         <f>RADIANS(F14)</f>
+        <v>0.26179938779914941</v>
+      </c>
+      <c r="G13" s="1">
+        <f>RADIANS(G14)</f>
         <v>0.52359877559829882</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" s="1">
+        <f>RADIANS(H14)</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="I13" s="1">
+        <f>RADIANS(I14)</f>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="J13" s="1">
+        <f>RADIANS(J14)</f>
+        <v>1.3089969389957472</v>
+      </c>
+      <c r="K13" s="1">
+        <f>RADIANS(K14)</f>
+        <v>1.5533430342749532</v>
+      </c>
+      <c r="L13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C14" s="26" t="s">
         <v>165</v>
       </c>
       <c r="D14" s="5">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="E14" t="s">
         <v>46</v>
       </c>
       <c r="F14" s="5">
+        <v>15</v>
+      </c>
+      <c r="G14" s="5">
         <v>30</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" s="5">
+        <v>45</v>
+      </c>
+      <c r="I14" s="5">
+        <v>60</v>
+      </c>
+      <c r="J14" s="5">
+        <v>75</v>
+      </c>
+      <c r="K14" s="5">
+        <v>89</v>
+      </c>
+      <c r="L14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C15" s="26" t="s">
         <v>164</v>
       </c>
@@ -15057,11 +16292,31 @@
         <f>ASIN((F2/(F2+F3)))</f>
         <v>0.53943938812170644</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="1">
+        <f>ASIN((G2/(G2+G3)))</f>
+        <v>0.53943938812170644</v>
+      </c>
+      <c r="H15" s="1">
+        <f>ASIN((H2/(H2+H3)))</f>
+        <v>0.53943938812170644</v>
+      </c>
+      <c r="I15" s="1">
+        <f>ASIN((I2/(I2+I3)))</f>
+        <v>0.53943938812170644</v>
+      </c>
+      <c r="J15" s="1">
+        <f>ASIN((J2/(J2+J3)))</f>
+        <v>0.53943938812170644</v>
+      </c>
+      <c r="K15" s="1">
+        <f>ASIN((K2/(K2+K3)))</f>
+        <v>0.53943938812170644</v>
+      </c>
+      <c r="L15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C16" s="26" t="s">
         <v>164</v>
       </c>
@@ -15076,113 +16331,237 @@
         <f t="shared" ref="F16" si="0">DEGREES(F15)</f>
         <v>30.907600242493331</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="2">
+        <f t="shared" ref="G16" si="1">DEGREES(G15)</f>
+        <v>30.907600242493331</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" ref="H16" si="2">DEGREES(H15)</f>
+        <v>30.907600242493331</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" ref="I16" si="3">DEGREES(I15)</f>
+        <v>30.907600242493331</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" ref="J16:K16" si="4">DEGREES(J15)</f>
+        <v>30.907600242493331</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="4"/>
+        <v>30.907600242493331</v>
+      </c>
+      <c r="L16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C17" s="26" t="s">
         <v>167</v>
       </c>
       <c r="D17" s="2">
         <f>ASIN(COS(D13)*SIN(D15))</f>
-        <v>0.7340592020747656</v>
+        <v>1.3500215170421661E-2</v>
       </c>
       <c r="E17" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="2">
         <f>ASIN(COS(F13)*SIN(F15))</f>
+        <v>0.51916196102910706</v>
+      </c>
+      <c r="G17" s="2">
+        <f>ASIN(COS(G13)*SIN(G15))</f>
         <v>0.46099374881500926</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" s="2">
+        <f>ASIN(COS(H13)*SIN(H15))</f>
+        <v>0.37170978574869223</v>
+      </c>
+      <c r="I17" s="2">
+        <f>ASIN(COS(I13)*SIN(I15))</f>
+        <v>0.25973819215339905</v>
+      </c>
+      <c r="J17" s="2">
+        <f>ASIN(COS(J13)*SIN(J15))</f>
+        <v>0.13333847083702191</v>
+      </c>
+      <c r="K17" s="2">
+        <f>ASIN(COS(K13)*SIN(K15))</f>
+        <v>8.9646371093753414E-3</v>
+      </c>
+      <c r="L17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C18" s="26" t="s">
         <v>167</v>
       </c>
       <c r="D18" s="2">
         <f>DEGREES(D17)</f>
-        <v>42.058494191624909</v>
+        <v>0.77350535178364854</v>
       </c>
       <c r="E18" t="s">
         <v>46</v>
       </c>
       <c r="F18" s="2">
         <f>DEGREES(F17)</f>
+        <v>29.745789250703154</v>
+      </c>
+      <c r="G18" s="2">
+        <f>DEGREES(G17)</f>
         <v>26.412996189014027</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" s="2">
+        <f>DEGREES(H17)</f>
+        <v>21.297401927112141</v>
+      </c>
+      <c r="I18" s="2">
+        <f>DEGREES(I17)</f>
+        <v>14.881902188747761</v>
+      </c>
+      <c r="J18" s="2">
+        <f>DEGREES(J17)</f>
+        <v>7.6397316256895644</v>
+      </c>
+      <c r="K18" s="2">
+        <f>DEGREES(K17)</f>
+        <v>0.51363587123356524</v>
+      </c>
+      <c r="L18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C19" s="26" t="s">
         <v>168</v>
       </c>
       <c r="D19" s="2">
         <f>RADIANS(90-D14-D18)</f>
-        <v>0.31313834912183214</v>
+        <v>3.9530773495216349E-3</v>
       </c>
       <c r="E19" t="s">
         <v>47</v>
       </c>
       <c r="F19" s="2">
         <f>RADIANS(90-F14-F18)</f>
+        <v>0.78983497796664015</v>
+      </c>
+      <c r="G19" s="2">
+        <f>RADIANS(90-G14-G18)</f>
         <v>0.58620380238158853</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" s="2">
+        <f>RADIANS(90-H14-H18)</f>
+        <v>0.41368837764875604</v>
+      </c>
+      <c r="I19" s="2">
+        <f>RADIANS(90-I14-I18)</f>
+        <v>0.26386058344489982</v>
+      </c>
+      <c r="J19" s="2">
+        <f>RADIANS(90-J14-J18)</f>
+        <v>0.12846091696212752</v>
+      </c>
+      <c r="K19" s="2">
+        <f>RADIANS(90-K14-K18)</f>
+        <v>8.4886554105679541E-3</v>
+      </c>
+      <c r="L19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C20" s="26" t="s">
         <v>168</v>
       </c>
       <c r="D20" s="2">
         <f>DEGREES(D19)</f>
-        <v>17.941505808375091</v>
+        <v>0.22649464821635146</v>
       </c>
       <c r="E20" t="s">
         <v>46</v>
       </c>
       <c r="F20" s="2">
         <f>DEGREES(F19)</f>
+        <v>45.254210749296846</v>
+      </c>
+      <c r="G20" s="2">
+        <f>DEGREES(G19)</f>
         <v>33.587003810985976</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" s="2">
+        <f>DEGREES(H19)</f>
+        <v>23.702598072887859</v>
+      </c>
+      <c r="I20" s="2">
+        <f>DEGREES(I19)</f>
+        <v>15.118097811252239</v>
+      </c>
+      <c r="J20" s="2">
+        <f>DEGREES(J19)</f>
+        <v>7.3602683743104356</v>
+      </c>
+      <c r="K20" s="2">
+        <f>DEGREES(K19)</f>
+        <v>0.48636412876643481</v>
+      </c>
+      <c r="L20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C21" s="26" t="s">
         <v>162</v>
       </c>
       <c r="D21" s="3">
         <f>D2*(SIN(D19)/SIN(D17))</f>
-        <v>631.36882882933344</v>
+        <v>402.04736497587606</v>
       </c>
       <c r="E21" t="s">
         <v>152</v>
       </c>
       <c r="F21" s="3">
         <f>F2*(SIN(F19)/SIN(F17))</f>
+        <v>1965.4343540051796</v>
+      </c>
+      <c r="G21" s="3">
+        <f>G2*(SIN(G19)/SIN(G17))</f>
         <v>1707.4678882558132</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" s="3">
+        <f>H2*(SIN(H19)/SIN(H17))</f>
+        <v>1519.5970667940214</v>
+      </c>
+      <c r="I21" s="3">
+        <f>I2*(SIN(I19)/SIN(I17))</f>
+        <v>1394.2873517775517</v>
+      </c>
+      <c r="J21" s="3">
+        <f>J2*(SIN(J19)/SIN(J17))</f>
+        <v>1323.0571940315779</v>
+      </c>
+      <c r="K21" s="3">
+        <f>K2*(SIN(K19)/SIN(K17))</f>
+        <v>1300.1017078232944</v>
+      </c>
+      <c r="L21" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="J23" s="32"/>
-    </row>
-    <row r="24" spans="3:19" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="O23" s="32"/>
+      <c r="V23" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" spans="3:24" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="26" t="s">
         <v>169</v>
       </c>
       <c r="D24" s="5">
+        <f>F24</f>
         <v>50</v>
       </c>
       <c r="E24" t="s">
@@ -15191,211 +16570,443 @@
       <c r="F24" s="5">
         <v>50</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="5">
+        <v>50</v>
+      </c>
+      <c r="H24" s="5">
+        <v>50</v>
+      </c>
+      <c r="I24" s="5">
+        <v>50</v>
+      </c>
+      <c r="J24" s="5">
+        <v>50</v>
+      </c>
+      <c r="K24" s="5">
+        <v>50</v>
+      </c>
+      <c r="L24" t="s">
         <v>170</v>
       </c>
-      <c r="Q24" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="25" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="V24" s="49" t="s">
+        <v>189</v>
+      </c>
+      <c r="W24" s="49"/>
+      <c r="X24" s="49"/>
+    </row>
+    <row r="25" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C25" s="26" t="s">
         <v>172</v>
       </c>
       <c r="D25" s="53">
-        <f>PI()*(D24/100)^2</f>
-        <v>0.78539816339744828</v>
+        <f>PI()*(D24/100/2)^2</f>
+        <v>0.19634954084936207</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="53">
-        <f>PI()*(F24/100)^2</f>
-        <v>0.78539816339744828</v>
-      </c>
-      <c r="G25" t="s">
+        <f>PI()*(F24/100/2)^2</f>
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="G25" s="53">
+        <f>PI()*(G24/100/2)^2</f>
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="H25" s="53">
+        <f>PI()*(H24/100/2)^2</f>
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="I25" s="53">
+        <f>PI()*(I24/100/2)^2</f>
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="J25" s="53">
+        <f>PI()*(J24/100/2)^2</f>
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="K25" s="53">
+        <f>PI()*(K24/100/2)^2</f>
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="L25" t="s">
         <v>1</v>
       </c>
-      <c r="H25" t="s">
+      <c r="M25" t="s">
         <v>174</v>
       </c>
-      <c r="Q25" s="49" t="s">
-        <v>190</v>
-      </c>
-      <c r="R25" s="49"/>
-      <c r="S25" s="49"/>
-    </row>
-    <row r="26" spans="3:19" ht="25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="3:24" ht="25" x14ac:dyDescent="0.35">
       <c r="C26" s="26" t="s">
         <v>171</v>
       </c>
       <c r="D26" s="51">
-        <f>PI()*(D24/100)^2*COS(RADIANS(90)-D13)</f>
-        <v>0.39269908169872403</v>
+        <f>PI()*(D24/100/2)^2*COS(RADIANS(90)-D13)</f>
+        <v>0.19631963586325035</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
       </c>
       <c r="F26" s="51">
-        <f>PI()*(F24/100)^2*COS(RADIANS(90)-F13)</f>
-        <v>0.39269908169872403</v>
-      </c>
-      <c r="G26" t="s">
+        <f>PI()*(F24/100/2)^2*COS(RADIANS(90)-F13)</f>
+        <v>5.081900066895028E-2</v>
+      </c>
+      <c r="G26" s="51">
+        <f>PI()*(G24/100/2)^2*COS(RADIANS(90)-G13)</f>
+        <v>9.8174770424681007E-2</v>
+      </c>
+      <c r="H26" s="51">
+        <f>PI()*(H24/100/2)^2*COS(RADIANS(90)-H13)</f>
+        <v>0.13884009181744894</v>
+      </c>
+      <c r="I26" s="51">
+        <f>PI()*(I24/100/2)^2*COS(RADIANS(90)-I13)</f>
+        <v>0.17004369039695791</v>
+      </c>
+      <c r="J26" s="51">
+        <f>PI()*(J24/100/2)^2*COS(RADIANS(90)-J13)</f>
+        <v>0.18965909248639923</v>
+      </c>
+      <c r="K26" s="51">
+        <f>PI()*(K24/100/2)^2*COS(RADIANS(90)-K13)</f>
+        <v>0.19631963586325035</v>
+      </c>
+      <c r="L26" t="s">
         <v>1</v>
       </c>
-      <c r="H26" s="54" t="s">
+      <c r="M26" s="54" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="28" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C28" s="26" t="s">
         <v>183</v>
       </c>
       <c r="D28" s="5">
-        <v>85</v>
+        <f>F28</f>
+        <v>100</v>
       </c>
       <c r="E28" t="s">
         <v>170</v>
       </c>
       <c r="F28" s="5">
-        <v>85</v>
-      </c>
-      <c r="G28" t="s">
+        <v>100</v>
+      </c>
+      <c r="G28" s="5">
+        <f>F28</f>
+        <v>100</v>
+      </c>
+      <c r="H28" s="5">
+        <f t="shared" ref="H28:K28" si="5">G28</f>
+        <v>100</v>
+      </c>
+      <c r="I28" s="5">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="J28" s="5">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="K28" s="5">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="L28" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C29" s="26" t="s">
         <v>184</v>
       </c>
       <c r="D29" s="52">
         <f>D28</f>
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="E29" s="52" t="s">
         <v>170</v>
       </c>
       <c r="F29" s="52">
         <f>F28</f>
-        <v>85</v>
-      </c>
-      <c r="G29" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" s="52">
+        <f>G28</f>
+        <v>100</v>
+      </c>
+      <c r="H29" s="52">
+        <f>H28</f>
+        <v>100</v>
+      </c>
+      <c r="I29" s="52">
+        <f>I28</f>
+        <v>100</v>
+      </c>
+      <c r="J29" s="52">
+        <f>J28</f>
+        <v>100</v>
+      </c>
+      <c r="K29" s="52">
+        <f>K28</f>
+        <v>100</v>
+      </c>
+      <c r="L29" t="s">
         <v>170</v>
       </c>
-      <c r="H29" t="s">
+      <c r="M29" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C30" s="26" t="s">
         <v>187</v>
       </c>
       <c r="D30" s="53">
-        <f>2*PI()*(D29/100/2)^2</f>
-        <v>1.1349003461093126</v>
+        <f>PI()*(D29/100/2)^2</f>
+        <v>0.78539816339744828</v>
       </c>
       <c r="E30" s="52" t="s">
         <v>1</v>
       </c>
       <c r="F30" s="53">
-        <f>2*PI()*(F29/100/2)^2</f>
-        <v>1.1349003461093126</v>
-      </c>
-      <c r="G30" t="s">
+        <f>PI()*(F29/100/2)^2</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="G30" s="53">
+        <f>PI()*(G29/100/2)^2</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="H30" s="53">
+        <f>PI()*(H29/100/2)^2</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="I30" s="53">
+        <f>PI()*(I29/100/2)^2</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="J30" s="53">
+        <f>PI()*(J29/100/2)^2</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="K30" s="53">
+        <f>PI()*(K29/100/2)^2</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="L30" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C32" s="26" t="s">
         <v>175</v>
       </c>
       <c r="D32">
         <f>(D29-D24)/2</f>
-        <v>17.5</v>
+        <v>25</v>
       </c>
       <c r="E32" t="s">
         <v>170</v>
       </c>
       <c r="F32">
         <f>(F29-F24)/2</f>
-        <v>17.5</v>
-      </c>
-      <c r="G32" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32">
+        <f>(G29-G24)/2</f>
+        <v>25</v>
+      </c>
+      <c r="H32">
+        <f>(H29-H24)/2</f>
+        <v>25</v>
+      </c>
+      <c r="I32">
+        <f>(I29-I24)/2</f>
+        <v>25</v>
+      </c>
+      <c r="J32">
+        <f>(J29-J24)/2</f>
+        <v>25</v>
+      </c>
+      <c r="K32">
+        <f>(K29-K24)/2</f>
+        <v>25</v>
+      </c>
+      <c r="L32" t="s">
         <v>170</v>
       </c>
-      <c r="H32" t="s">
+      <c r="M32" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C34" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D34" s="1">
         <f>ATAN((D32/100)/(D21*1000))*10000000</f>
-        <v>2.7717554622466181</v>
+        <v>6.2181728268501022</v>
       </c>
       <c r="E34" t="s">
         <v>178</v>
       </c>
       <c r="F34" s="1">
         <f>ATAN((F32/100)/(F21*1000))*10000000</f>
-        <v>1.0249094650837782</v>
-      </c>
-      <c r="G34" t="s">
+        <v>1.2719834650826491</v>
+      </c>
+      <c r="G34" s="1">
+        <f>ATAN((G32/100)/(G21*1000))*10000000</f>
+        <v>1.4641563786911063</v>
+      </c>
+      <c r="H34" s="1">
+        <f>ATAN((H32/100)/(H21*1000))*10000000</f>
+        <v>1.6451729571144584</v>
+      </c>
+      <c r="I34" s="1">
+        <f>ATAN((I32/100)/(I21*1000))*10000000</f>
+        <v>1.79303068109509</v>
+      </c>
+      <c r="J34" s="1">
+        <f>ATAN((J32/100)/(J21*1000))*10000000</f>
+        <v>1.8895630599173494</v>
+      </c>
+      <c r="K34" s="1">
+        <f>ATAN((K32/100)/(K21*1000))*10000000</f>
+        <v>1.9229264794872194</v>
+      </c>
+      <c r="L34" t="s">
         <v>178</v>
       </c>
-      <c r="H34" t="s">
+      <c r="M34" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="35" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C35" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="D35" s="1">
+        <v>191</v>
+      </c>
+      <c r="D35" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="F35" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="G35" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="H35" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="I35" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="J35" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="K35" s="55">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="36" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C36" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="D36" s="1">
         <f>D26/D30</f>
-        <v>0.34602076124567471</v>
-      </c>
-      <c r="F35" s="1">
+        <v>0.24996192378909782</v>
+      </c>
+      <c r="F36" s="1">
         <f>F26/F30</f>
-        <v>0.34602076124567471</v>
-      </c>
-      <c r="H35" t="s">
+        <v>6.4704761275630185E-2</v>
+      </c>
+      <c r="G36" s="1">
+        <f>G26/G30</f>
+        <v>0.12499999999999996</v>
+      </c>
+      <c r="H36" s="1">
+        <f>H26/H30</f>
+        <v>0.17677669529663689</v>
+      </c>
+      <c r="I36" s="1">
+        <f>I26/I30</f>
+        <v>0.21650635094610965</v>
+      </c>
+      <c r="J36" s="1">
+        <f>J26/J30</f>
+        <v>0.24148145657226708</v>
+      </c>
+      <c r="K36" s="1">
+        <f>K26/K30</f>
+        <v>0.24996192378909782</v>
+      </c>
+      <c r="M36" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="M40" t="s">
+    <row r="37" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C37" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="D37" s="1">
+        <f>D36*D35</f>
+        <v>9.998476951563913E-2</v>
+      </c>
+      <c r="F37" s="1">
+        <f>F36*F35</f>
+        <v>2.5881904510252074E-2</v>
+      </c>
+      <c r="G37" s="1">
+        <f>G36*G35</f>
+        <v>4.9999999999999989E-2</v>
+      </c>
+      <c r="H37" s="1">
+        <f>H36*H35</f>
+        <v>7.0710678118654766E-2</v>
+      </c>
+      <c r="I37" s="1">
+        <f>I36*I35</f>
+        <v>8.6602540378443865E-2</v>
+      </c>
+      <c r="J37" s="1">
+        <f>J36*J35</f>
+        <v>9.659258262890684E-2</v>
+      </c>
+      <c r="K37" s="1">
+        <f>K36*K35</f>
+        <v>9.998476951563913E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="R41" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="41" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="I41" t="s">
+    <row r="42" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="N42" t="s">
         <v>175</v>
       </c>
-      <c r="N41" t="s">
+      <c r="S42" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="L42" t="s">
+    <row r="43" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="Q43" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="K43" t="s">
+    <row r="44" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P44" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="45" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="J45" t="s">
+    <row r="46" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="O46" t="s">
         <v>181</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="Q25:S25"/>
+    <mergeCell ref="V24:X24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
updated trade tree excel with pointing eff acc
</commit_message>
<xml_diff>
--- a/CCP Trade Tree Analysis.xlsx
+++ b/CCP Trade Tree Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuitenbr/Desktop/lunarspark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E9B94D-A9FE-F740-A32B-6E4740B49948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A648746-FB78-384C-AACF-FB0F5BBD7AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1280" windowWidth="33800" windowHeight="21120" activeTab="4" xr2:uid="{0D0644B8-F9A6-4A61-A91E-2BD3522A7E9F}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="196">
   <si>
     <t>solar array size</t>
   </si>
@@ -657,6 +657,12 @@
   </si>
   <si>
     <t>overall adjusted eff</t>
+  </si>
+  <si>
+    <t>TODO: Add average duty cycle percentage</t>
+  </si>
+  <si>
+    <t>select 45 deg</t>
   </si>
 </sst>
 </file>
@@ -3524,54 +3530,60 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Pointing Eff Acc'!$F$14:$K$14</c:f>
+              <c:f>'Pointing Eff Acc'!$F$14:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89</c:v>
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pointing Eff Acc'!$F$36:$K$36</c:f>
+              <c:f>'Pointing Eff Acc'!$F$36:$L$36</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6.4704761275630185E-2</c:v>
+                  <c:v>9.9978246375051177E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12499999999999996</c:v>
+                  <c:v>0.19483162079514554</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17677669529663689</c:v>
+                  <c:v>0.27969795157770555</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.21650635094610965</c:v>
+                  <c:v>0.35022700160298753</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.24148145657226708</c:v>
+                  <c:v>0.40280346090517777</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.24996192378909782</c:v>
+                  <c:v>0.43473226699280249</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.44437675340284055</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3611,54 +3623,60 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Pointing Eff Acc'!$F$14:$K$14</c:f>
+              <c:f>'Pointing Eff Acc'!$F$14:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89</c:v>
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pointing Eff Acc'!$F$37:$K$37</c:f>
+              <c:f>'Pointing Eff Acc'!$F$37:$L$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.5881904510252074E-2</c:v>
+                  <c:v>3.9991298550020475E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9999999999999989E-2</c:v>
+                  <c:v>7.7932648318058226E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0710678118654766E-2</c:v>
+                  <c:v>0.11187918063108222</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.6602540378443865E-2</c:v>
+                  <c:v>0.14009080064119503</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.659258262890684E-2</c:v>
+                  <c:v>0.16112138436207113</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.998476951563913E-2</c:v>
+                  <c:v>0.17389290679712099</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.17775070136113624</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7125,13 +7143,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>182880</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>172720</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>132080</xdr:rowOff>
@@ -7188,13 +7206,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>82066</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>728980</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>27939</xdr:rowOff>
@@ -7232,13 +7250,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>274320</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>144271</xdr:rowOff>
@@ -7276,13 +7294,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>91440</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>175602</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>424180</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>2539</xdr:rowOff>
@@ -7320,13 +7338,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>81280</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>186112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>165099</xdr:rowOff>
@@ -7364,13 +7382,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>422174</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>162560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>721772</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>116840</xdr:rowOff>
@@ -7425,13 +7443,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>325120</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>142240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>10160</xdr:rowOff>
@@ -7491,13 +7509,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>558800</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>20320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>802640</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>10160</xdr:rowOff>
@@ -7554,13 +7572,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>81280</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>71120</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>81280</xdr:rowOff>
@@ -7617,13 +7635,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>223520</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>751840</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
@@ -7689,7 +7707,7 @@
       <xdr:rowOff>10160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>421640</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -12043,8 +12061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB1BC88-0916-3A47-BF9E-DDA64C4AACEA}">
   <dimension ref="B1:P21"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12394,6 +12412,9 @@
       <c r="N10">
         <f t="shared" si="2"/>
         <v>488</v>
+      </c>
+      <c r="P10" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
@@ -15984,21 +16005,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1EB7CC8-2E43-AD42-9797-36D0C73BF74C}">
-  <dimension ref="C2:X46"/>
+  <dimension ref="B2:Y46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="N51" sqref="N51"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" customWidth="1"/>
-    <col min="6" max="11" width="8.1640625" customWidth="1"/>
-    <col min="12" max="12" width="5.1640625" customWidth="1"/>
+    <col min="6" max="12" width="8.1640625" customWidth="1"/>
+    <col min="13" max="13" width="5.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C2" s="26" t="s">
         <v>163</v>
       </c>
@@ -16026,11 +16047,14 @@
       <c r="K2">
         <v>1373</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2">
+        <v>1373</v>
+      </c>
+      <c r="M2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="26" t="s">
         <v>166</v>
       </c>
@@ -16058,19 +16082,22 @@
       <c r="K3" s="5">
         <v>1300</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="5">
+        <v>1300</v>
+      </c>
+      <c r="M3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="26"/>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="26" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="26" t="s">
         <v>158</v>
       </c>
@@ -16098,11 +16125,14 @@
       <c r="K6">
         <v>12</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6">
+        <v>12</v>
+      </c>
+      <c r="M6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="26" t="s">
         <v>159</v>
       </c>
@@ -16130,19 +16160,22 @@
       <c r="K7">
         <v>90</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7">
+        <v>90</v>
+      </c>
+      <c r="M7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="26"/>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="26" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C10" s="26" t="s">
         <v>158</v>
       </c>
@@ -16170,11 +16203,14 @@
       <c r="K10">
         <v>12</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10">
+        <v>12</v>
+      </c>
+      <c r="M10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="26" t="s">
         <v>159</v>
       </c>
@@ -16202,11 +16238,14 @@
       <c r="K11">
         <v>67</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11">
+        <v>67</v>
+      </c>
+      <c r="M11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="26" t="s">
         <v>165</v>
       </c>
@@ -16219,33 +16258,37 @@
       </c>
       <c r="F13" s="1">
         <f>RADIANS(F14)</f>
-        <v>0.26179938779914941</v>
+        <v>0.22689280275926285</v>
       </c>
       <c r="G13" s="1">
         <f>RADIANS(G14)</f>
-        <v>0.52359877559829882</v>
+        <v>0.4537856055185257</v>
       </c>
       <c r="H13" s="1">
         <f>RADIANS(H14)</f>
-        <v>0.78539816339744828</v>
+        <v>0.68067840827778847</v>
       </c>
       <c r="I13" s="1">
         <f>RADIANS(I14)</f>
-        <v>1.0471975511965976</v>
+        <v>0.90757121103705141</v>
       </c>
       <c r="J13" s="1">
         <f>RADIANS(J14)</f>
-        <v>1.3089969389957472</v>
+        <v>1.1344640137963142</v>
       </c>
       <c r="K13" s="1">
         <f>RADIANS(K14)</f>
-        <v>1.5533430342749532</v>
-      </c>
-      <c r="L13" t="s">
+        <v>1.3613568165555769</v>
+      </c>
+      <c r="L13" s="1">
+        <f>RADIANS(L14)</f>
+        <v>1.5882496193148399</v>
+      </c>
+      <c r="M13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" s="26" t="s">
         <v>165</v>
       </c>
@@ -16256,28 +16299,37 @@
         <v>46</v>
       </c>
       <c r="F14" s="5">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G14" s="5">
-        <v>30</v>
+        <f>F14+$F14</f>
+        <v>26</v>
       </c>
       <c r="H14" s="5">
-        <v>45</v>
+        <f t="shared" ref="H14:L14" si="0">G14+$F14</f>
+        <v>39</v>
       </c>
       <c r="I14" s="5">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>52</v>
       </c>
       <c r="J14" s="5">
-        <v>75</v>
+        <f t="shared" si="0"/>
+        <v>65</v>
       </c>
       <c r="K14" s="5">
-        <v>89</v>
-      </c>
-      <c r="L14" t="s">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="L14" s="5">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="M14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="26" t="s">
         <v>164</v>
       </c>
@@ -16312,11 +16364,15 @@
         <f>ASIN((K2/(K2+K3)))</f>
         <v>0.53943938812170644</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="1">
+        <f>ASIN((L2/(L2+L3)))</f>
+        <v>0.53943938812170644</v>
+      </c>
+      <c r="M15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" s="26" t="s">
         <v>164</v>
       </c>
@@ -16328,34 +16384,38 @@
         <v>46</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" ref="F16" si="0">DEGREES(F15)</f>
+        <f t="shared" ref="F16" si="1">DEGREES(F15)</f>
         <v>30.907600242493331</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" ref="G16" si="1">DEGREES(G15)</f>
+        <f t="shared" ref="G16" si="2">DEGREES(G15)</f>
         <v>30.907600242493331</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" ref="H16" si="2">DEGREES(H15)</f>
+        <f t="shared" ref="H16" si="3">DEGREES(H15)</f>
         <v>30.907600242493331</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" ref="I16" si="3">DEGREES(I15)</f>
+        <f t="shared" ref="I16" si="4">DEGREES(I15)</f>
         <v>30.907600242493331</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" ref="J16:K16" si="4">DEGREES(J15)</f>
+        <f t="shared" ref="J16:L16" si="5">DEGREES(J15)</f>
         <v>30.907600242493331</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30.907600242493331</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="2">
+        <f t="shared" si="5"/>
+        <v>30.907600242493331</v>
+      </c>
+      <c r="M16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C17" s="26" t="s">
         <v>167</v>
       </c>
@@ -16368,33 +16428,37 @@
       </c>
       <c r="F17" s="2">
         <f>ASIN(COS(F13)*SIN(F15))</f>
-        <v>0.51916196102910706</v>
+        <v>0.5241648134856125</v>
       </c>
       <c r="G17" s="2">
         <f>ASIN(COS(G13)*SIN(G15))</f>
-        <v>0.46099374881500926</v>
+        <v>0.47987705229094135</v>
       </c>
       <c r="H17" s="2">
         <f>ASIN(COS(H13)*SIN(H15))</f>
-        <v>0.37170978574869223</v>
+        <v>0.41062773976496941</v>
       </c>
       <c r="I17" s="2">
         <f>ASIN(COS(I13)*SIN(I15))</f>
-        <v>0.25973819215339905</v>
+        <v>0.32176096010212818</v>
       </c>
       <c r="J17" s="2">
         <f>ASIN(COS(J13)*SIN(J15))</f>
-        <v>0.13333847083702191</v>
+        <v>0.21882215135884239</v>
       </c>
       <c r="K17" s="2">
         <f>ASIN(COS(K13)*SIN(K15))</f>
-        <v>8.9646371093753414E-3</v>
-      </c>
-      <c r="L17" t="s">
+        <v>0.10699894488840596</v>
+      </c>
+      <c r="L17" s="2">
+        <f>ASIN(COS(L13)*SIN(L15))</f>
+        <v>-8.9646371093752789E-3</v>
+      </c>
+      <c r="M17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C18" s="26" t="s">
         <v>167</v>
       </c>
@@ -16407,33 +16471,37 @@
       </c>
       <c r="F18" s="2">
         <f>DEGREES(F17)</f>
-        <v>29.745789250703154</v>
+        <v>30.032431581987574</v>
       </c>
       <c r="G18" s="2">
         <f>DEGREES(G17)</f>
-        <v>26.412996189014027</v>
+        <v>27.494929781449652</v>
       </c>
       <c r="H18" s="2">
         <f>DEGREES(H17)</f>
-        <v>21.297401927112141</v>
+        <v>23.527236439529034</v>
       </c>
       <c r="I18" s="2">
         <f>DEGREES(I17)</f>
-        <v>14.881902188747761</v>
+        <v>18.435545025929216</v>
       </c>
       <c r="J18" s="2">
         <f>DEGREES(J17)</f>
-        <v>7.6397316256895644</v>
+        <v>12.537585736834561</v>
       </c>
       <c r="K18" s="2">
         <f>DEGREES(K17)</f>
-        <v>0.51363587123356524</v>
-      </c>
-      <c r="L18" t="s">
+        <v>6.1305879544585551</v>
+      </c>
+      <c r="L18" s="2">
+        <f>DEGREES(L17)</f>
+        <v>-0.51363587123356169</v>
+      </c>
+      <c r="M18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C19" s="26" t="s">
         <v>168</v>
       </c>
@@ -16446,33 +16514,37 @@
       </c>
       <c r="F19" s="2">
         <f>RADIANS(90-F14-F18)</f>
-        <v>0.78983497796664015</v>
+        <v>0.81973871055002123</v>
       </c>
       <c r="G19" s="2">
         <f>RADIANS(90-G14-G18)</f>
-        <v>0.58620380238158853</v>
+        <v>0.63713366898542945</v>
       </c>
       <c r="H19" s="2">
         <f>RADIANS(90-H14-H18)</f>
-        <v>0.41368837764875604</v>
+        <v>0.47949017875213867</v>
       </c>
       <c r="I19" s="2">
         <f>RADIANS(90-I14-I18)</f>
-        <v>0.26386058344489982</v>
+        <v>0.34146415565571703</v>
       </c>
       <c r="J19" s="2">
         <f>RADIANS(90-J14-J18)</f>
-        <v>0.12846091696212752</v>
+        <v>0.21751016163973999</v>
       </c>
       <c r="K19" s="2">
         <f>RADIANS(90-K14-K18)</f>
-        <v>8.4886554105679541E-3</v>
-      </c>
-      <c r="L19" t="s">
+        <v>0.10244056535091357</v>
+      </c>
+      <c r="L19" s="2">
+        <f>RADIANS(90-L14-L18)</f>
+        <v>-8.4886554105680148E-3</v>
+      </c>
+      <c r="M19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C20" s="26" t="s">
         <v>168</v>
       </c>
@@ -16485,33 +16557,37 @@
       </c>
       <c r="F20" s="2">
         <f>DEGREES(F19)</f>
-        <v>45.254210749296846</v>
+        <v>46.967568418012426</v>
       </c>
       <c r="G20" s="2">
         <f>DEGREES(G19)</f>
-        <v>33.587003810985976</v>
+        <v>36.505070218550344</v>
       </c>
       <c r="H20" s="2">
         <f>DEGREES(H19)</f>
-        <v>23.702598072887859</v>
+        <v>27.47276356047097</v>
       </c>
       <c r="I20" s="2">
         <f>DEGREES(I19)</f>
-        <v>15.118097811252239</v>
+        <v>19.564454974070784</v>
       </c>
       <c r="J20" s="2">
         <f>DEGREES(J19)</f>
-        <v>7.3602683743104356</v>
+        <v>12.462414263165439</v>
       </c>
       <c r="K20" s="2">
         <f>DEGREES(K19)</f>
-        <v>0.48636412876643481</v>
-      </c>
-      <c r="L20" t="s">
+        <v>5.8694120455414449</v>
+      </c>
+      <c r="L20" s="2">
+        <f>DEGREES(L19)</f>
+        <v>-0.48636412876643825</v>
+      </c>
+      <c r="M20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C21" s="26" t="s">
         <v>162</v>
       </c>
@@ -16524,39 +16600,43 @@
       </c>
       <c r="F21" s="3">
         <f>F2*(SIN(F19)/SIN(F17))</f>
-        <v>1965.4343540051796</v>
+        <v>2005.2712262622533</v>
       </c>
       <c r="G21" s="3">
         <f>G2*(SIN(G19)/SIN(G17))</f>
-        <v>1707.4678882558132</v>
+        <v>1769.2055848785083</v>
       </c>
       <c r="H21" s="3">
         <f>H2*(SIN(H19)/SIN(H17))</f>
-        <v>1519.5970667940214</v>
+        <v>1586.737733631941</v>
       </c>
       <c r="I21" s="3">
         <f>I2*(SIN(I19)/SIN(I17))</f>
-        <v>1394.2873517775517</v>
+        <v>1453.8828951480778</v>
       </c>
       <c r="J21" s="3">
         <f>J2*(SIN(J19)/SIN(J17))</f>
-        <v>1323.0571940315779</v>
+        <v>1364.8985526636545</v>
       </c>
       <c r="K21" s="3">
         <f>K2*(SIN(K19)/SIN(K17))</f>
-        <v>1300.1017078232944</v>
-      </c>
-      <c r="L21" t="s">
+        <v>1314.7166503092596</v>
+      </c>
+      <c r="L21" s="3">
+        <f>L2*(SIN(L19)/SIN(L17))</f>
+        <v>1300.1017078233126</v>
+      </c>
+      <c r="M21" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="O23" s="32"/>
-      <c r="V23" t="s">
+    <row r="23" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="P23" s="32"/>
+      <c r="W23" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="3:24" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:25" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="26" t="s">
         <v>169</v>
       </c>
@@ -16585,16 +16665,19 @@
       <c r="K24" s="5">
         <v>50</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" s="5">
+        <v>50</v>
+      </c>
+      <c r="M24" t="s">
         <v>170</v>
       </c>
-      <c r="V24" s="49" t="s">
+      <c r="W24" s="49" t="s">
         <v>189</v>
       </c>
-      <c r="W24" s="49"/>
       <c r="X24" s="49"/>
-    </row>
-    <row r="25" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="Y24" s="49"/>
+    </row>
+    <row r="25" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C25" s="26" t="s">
         <v>172</v>
       </c>
@@ -16629,14 +16712,18 @@
         <f>PI()*(K24/100/2)^2</f>
         <v>0.19634954084936207</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" s="53">
+        <f>PI()*(L24/100/2)^2</f>
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="M25" t="s">
         <v>1</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="3:24" ht="25" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:25" ht="25" x14ac:dyDescent="0.35">
       <c r="C26" s="26" t="s">
         <v>171</v>
       </c>
@@ -16649,239 +16736,263 @@
       </c>
       <c r="F26" s="51">
         <f>PI()*(F24/100/2)^2*COS(RADIANS(90)-F13)</f>
-        <v>5.081900066895028E-2</v>
+        <v>4.4169036233997816E-2</v>
       </c>
       <c r="G26" s="51">
         <f>PI()*(G24/100/2)^2*COS(RADIANS(90)-G13)</f>
-        <v>9.8174770424681007E-2</v>
+        <v>8.6073973393643657E-2</v>
       </c>
       <c r="H26" s="51">
         <f>PI()*(H24/100/2)^2*COS(RADIANS(90)-H13)</f>
-        <v>0.13884009181744894</v>
+        <v>0.12356676982977657</v>
       </c>
       <c r="I26" s="51">
         <f>PI()*(I24/100/2)^2*COS(RADIANS(90)-I13)</f>
-        <v>0.17004369039695791</v>
+        <v>0.15472554965503965</v>
       </c>
       <c r="J26" s="51">
         <f>PI()*(J24/100/2)^2*COS(RADIANS(90)-J13)</f>
-        <v>0.18965909248639923</v>
+        <v>0.17795311785284765</v>
       </c>
       <c r="K26" s="51">
         <f>PI()*(K24/100/2)^2*COS(RADIANS(90)-K13)</f>
+        <v>0.19205883228698786</v>
+      </c>
+      <c r="L26" s="51">
+        <f>PI()*(L24/100/2)^2*COS(RADIANS(90)-L13)</f>
         <v>0.19631963586325035</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>1</v>
       </c>
-      <c r="M26" s="54" t="s">
+      <c r="N26" s="54" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="28" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C28" s="26" t="s">
         <v>183</v>
       </c>
       <c r="D28" s="5">
         <f>F28</f>
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="E28" t="s">
         <v>170</v>
       </c>
       <c r="F28" s="5">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="G28" s="5">
         <f>F28</f>
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="H28" s="5">
-        <f t="shared" ref="H28:K28" si="5">G28</f>
-        <v>100</v>
+        <f t="shared" ref="H28:K28" si="6">G28</f>
+        <v>75</v>
       </c>
       <c r="I28" s="5">
-        <f t="shared" si="5"/>
-        <v>100</v>
+        <f t="shared" si="6"/>
+        <v>75</v>
       </c>
       <c r="J28" s="5">
-        <f t="shared" si="5"/>
-        <v>100</v>
+        <f t="shared" si="6"/>
+        <v>75</v>
       </c>
       <c r="K28" s="5">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="L28" t="s">
+        <f t="shared" si="6"/>
+        <v>75</v>
+      </c>
+      <c r="L28" s="5">
+        <f t="shared" ref="L28" si="7">K28</f>
+        <v>75</v>
+      </c>
+      <c r="M28" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C29" s="26" t="s">
         <v>184</v>
       </c>
       <c r="D29" s="52">
         <f>D28</f>
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="E29" s="52" t="s">
         <v>170</v>
       </c>
       <c r="F29" s="52">
         <f>F28</f>
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="G29" s="52">
         <f>G28</f>
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="H29" s="52">
         <f>H28</f>
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="I29" s="52">
         <f>I28</f>
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J29" s="52">
         <f>J28</f>
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="K29" s="52">
         <f>K28</f>
-        <v>100</v>
-      </c>
-      <c r="L29" t="s">
+        <v>75</v>
+      </c>
+      <c r="L29" s="52">
+        <f>L28</f>
+        <v>75</v>
+      </c>
+      <c r="M29" t="s">
         <v>170</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C30" s="26" t="s">
         <v>187</v>
       </c>
       <c r="D30" s="53">
         <f>PI()*(D29/100/2)^2</f>
-        <v>0.78539816339744828</v>
+        <v>0.44178646691106466</v>
       </c>
       <c r="E30" s="52" t="s">
         <v>1</v>
       </c>
       <c r="F30" s="53">
         <f>PI()*(F29/100/2)^2</f>
-        <v>0.78539816339744828</v>
+        <v>0.44178646691106466</v>
       </c>
       <c r="G30" s="53">
         <f>PI()*(G29/100/2)^2</f>
-        <v>0.78539816339744828</v>
+        <v>0.44178646691106466</v>
       </c>
       <c r="H30" s="53">
         <f>PI()*(H29/100/2)^2</f>
-        <v>0.78539816339744828</v>
+        <v>0.44178646691106466</v>
       </c>
       <c r="I30" s="53">
         <f>PI()*(I29/100/2)^2</f>
-        <v>0.78539816339744828</v>
+        <v>0.44178646691106466</v>
       </c>
       <c r="J30" s="53">
         <f>PI()*(J29/100/2)^2</f>
-        <v>0.78539816339744828</v>
+        <v>0.44178646691106466</v>
       </c>
       <c r="K30" s="53">
         <f>PI()*(K29/100/2)^2</f>
-        <v>0.78539816339744828</v>
-      </c>
-      <c r="L30" t="s">
+        <v>0.44178646691106466</v>
+      </c>
+      <c r="L30" s="53">
+        <f>PI()*(L29/100/2)^2</f>
+        <v>0.44178646691106466</v>
+      </c>
+      <c r="M30" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C32" s="26" t="s">
         <v>175</v>
       </c>
       <c r="D32">
         <f>(D29-D24)/2</f>
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E32" t="s">
         <v>170</v>
       </c>
       <c r="F32">
         <f>(F29-F24)/2</f>
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="G32">
         <f>(G29-G24)/2</f>
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="H32">
         <f>(H29-H24)/2</f>
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="I32">
         <f>(I29-I24)/2</f>
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="J32">
         <f>(J29-J24)/2</f>
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="K32">
         <f>(K29-K24)/2</f>
-        <v>25</v>
-      </c>
-      <c r="L32" t="s">
+        <v>12.5</v>
+      </c>
+      <c r="L32">
+        <f>(L29-L24)/2</f>
+        <v>12.5</v>
+      </c>
+      <c r="M32" t="s">
         <v>170</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C34" s="26" t="s">
         <v>188</v>
       </c>
       <c r="D34" s="1">
         <f>ATAN((D32/100)/(D21*1000))*10000000</f>
-        <v>6.2181728268501022</v>
+        <v>3.1090864134253517</v>
       </c>
       <c r="E34" t="s">
         <v>178</v>
       </c>
       <c r="F34" s="1">
         <f>ATAN((F32/100)/(F21*1000))*10000000</f>
-        <v>1.2719834650826491</v>
+        <v>0.62335707191587697</v>
       </c>
       <c r="G34" s="1">
         <f>ATAN((G32/100)/(G21*1000))*10000000</f>
-        <v>1.4641563786911063</v>
+        <v>0.70653179635188401</v>
       </c>
       <c r="H34" s="1">
         <f>ATAN((H32/100)/(H21*1000))*10000000</f>
-        <v>1.6451729571144584</v>
+        <v>0.7877798413092677</v>
       </c>
       <c r="I34" s="1">
         <f>ATAN((I32/100)/(I21*1000))*10000000</f>
-        <v>1.79303068109509</v>
+        <v>0.85976663194230962</v>
       </c>
       <c r="J34" s="1">
         <f>ATAN((J32/100)/(J21*1000))*10000000</f>
-        <v>1.8895630599173494</v>
+        <v>0.91581897977734039</v>
       </c>
       <c r="K34" s="1">
         <f>ATAN((K32/100)/(K21*1000))*10000000</f>
-        <v>1.9229264794872194</v>
-      </c>
-      <c r="L34" t="s">
+        <v>0.95077521054134351</v>
+      </c>
+      <c r="L34" s="1">
+        <f>ATAN((L32/100)/(L21*1000))*10000000</f>
+        <v>0.96146323974360526</v>
+      </c>
+      <c r="M34" t="s">
         <v>178</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="35" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C35" s="26" t="s">
         <v>191</v>
       </c>
@@ -16906,107 +17017,123 @@
       <c r="K35" s="55">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="36" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="L35" s="55">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C36" s="26" t="s">
         <v>192</v>
       </c>
       <c r="D36" s="1">
         <f>D26/D30</f>
-        <v>0.24996192378909782</v>
+        <v>0.44437675340284055</v>
       </c>
       <c r="F36" s="1">
         <f>F26/F30</f>
-        <v>6.4704761275630185E-2</v>
+        <v>9.9978246375051177E-2</v>
       </c>
       <c r="G36" s="1">
         <f>G26/G30</f>
-        <v>0.12499999999999996</v>
+        <v>0.19483162079514554</v>
       </c>
       <c r="H36" s="1">
         <f>H26/H30</f>
-        <v>0.17677669529663689</v>
+        <v>0.27969795157770555</v>
       </c>
       <c r="I36" s="1">
         <f>I26/I30</f>
-        <v>0.21650635094610965</v>
+        <v>0.35022700160298753</v>
       </c>
       <c r="J36" s="1">
         <f>J26/J30</f>
-        <v>0.24148145657226708</v>
+        <v>0.40280346090517777</v>
       </c>
       <c r="K36" s="1">
         <f>K26/K30</f>
-        <v>0.24996192378909782</v>
-      </c>
-      <c r="M36" t="s">
+        <v>0.43473226699280249</v>
+      </c>
+      <c r="L36" s="1">
+        <f>L26/L30</f>
+        <v>0.44437675340284055</v>
+      </c>
+      <c r="N36" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="37" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C37" s="26" t="s">
         <v>193</v>
       </c>
       <c r="D37" s="1">
         <f>D36*D35</f>
-        <v>9.998476951563913E-2</v>
+        <v>0.17775070136113624</v>
       </c>
       <c r="F37" s="1">
         <f>F36*F35</f>
-        <v>2.5881904510252074E-2</v>
+        <v>3.9991298550020475E-2</v>
       </c>
       <c r="G37" s="1">
         <f>G36*G35</f>
-        <v>4.9999999999999989E-2</v>
+        <v>7.7932648318058226E-2</v>
       </c>
       <c r="H37" s="1">
         <f>H36*H35</f>
-        <v>7.0710678118654766E-2</v>
+        <v>0.11187918063108222</v>
       </c>
       <c r="I37" s="1">
         <f>I36*I35</f>
-        <v>8.6602540378443865E-2</v>
+        <v>0.14009080064119503</v>
       </c>
       <c r="J37" s="1">
         <f>J36*J35</f>
-        <v>9.659258262890684E-2</v>
+        <v>0.16112138436207113</v>
       </c>
       <c r="K37" s="1">
         <f>K36*K35</f>
-        <v>9.998476951563913E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="R41" t="s">
+        <v>0.17389290679712099</v>
+      </c>
+      <c r="L37" s="1">
+        <f>L36*L35</f>
+        <v>0.17775070136113624</v>
+      </c>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="S41" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="42" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="N42" t="s">
+    <row r="42" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="O42" t="s">
         <v>175</v>
       </c>
-      <c r="S42" t="s">
+      <c r="T42" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="43" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="Q43" t="s">
+    <row r="43" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="R43" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="44" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="P44" t="s">
+    <row r="44" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="Q44" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="46" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="O46" t="s">
+    <row r="45" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="P46" t="s">
         <v>181</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="V24:X24"/>
+    <mergeCell ref="W24:Y24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>